<commit_message>
Fixed power off and serial out issues
</commit_message>
<xml_diff>
--- a/Documentation/KSP Controller Design Data.xlsx
+++ b/Documentation/KSP Controller Design Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="11310" windowHeight="5430" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="11310" windowHeight="5430" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="447">
   <si>
     <t>M</t>
   </si>
@@ -1430,6 +1430,9 @@
   </si>
   <si>
     <t>not yet supported, krpc issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added an explicit light off </t>
   </si>
 </sst>
 </file>
@@ -1713,8 +1716,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142046008"/>
-        <c:axId val="142045616"/>
+        <c:axId val="142205784"/>
+        <c:axId val="142202256"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1797,11 +1800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142048752"/>
-        <c:axId val="142049928"/>
+        <c:axId val="142206176"/>
+        <c:axId val="142203432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142046008"/>
+        <c:axId val="142205784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,12 +1861,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142045616"/>
+        <c:crossAx val="142202256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142045616"/>
+        <c:axId val="142202256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1920,12 +1923,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142046008"/>
+        <c:crossAx val="142205784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142049928"/>
+        <c:axId val="142203432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1971,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142048752"/>
+        <c:crossAx val="142206176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142048752"/>
+        <c:axId val="142206176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,7 +1986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142049928"/>
+        <c:crossAx val="142203432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2079,6 +2082,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5264,11 +5268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142050320"/>
-        <c:axId val="142051104"/>
+        <c:axId val="142201080"/>
+        <c:axId val="142204216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142050320"/>
+        <c:axId val="142201080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5325,12 +5329,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142051104"/>
+        <c:crossAx val="142204216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142051104"/>
+        <c:axId val="142204216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5387,7 +5391,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142050320"/>
+        <c:crossAx val="142201080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5401,6 +5405,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8089,7 +8094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -12655,9 +12660,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -13631,7 +13636,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -13648,7 +13653,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -13662,7 +13667,10 @@
         <v>400</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>412</v>
+        <v>277</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update do design notes
</commit_message>
<xml_diff>
--- a/Documentation/KSP Controller Design Data.xlsx
+++ b/Documentation/KSP Controller Design Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="11310" windowHeight="5430" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="11310" windowHeight="5430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -1422,17 +1422,17 @@
     <t>All errors fixed, writes to the GUI message area</t>
   </si>
   <si>
-    <t>orbital selection constantly sets chase for planes??
+    <t>Structure done but needs naming convention clean up, review of globals etc</t>
+  </si>
+  <si>
+    <t>not yet supported, krpc issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added an explicit light off </t>
+  </si>
+  <si>
+    <t>orbital selection constantly sets chase for planes, this is due to a lack of velocity data, need to filter this
 default distance only works after some time, needs krpc fix. Hack installed to hold cam distance for timer</t>
-  </si>
-  <si>
-    <t>Structure done but needs naming convention clean up, review of globals etc</t>
-  </si>
-  <si>
-    <t>not yet supported, krpc issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added an explicit light off </t>
   </si>
 </sst>
 </file>
@@ -1716,8 +1716,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142205784"/>
-        <c:axId val="142202256"/>
+        <c:axId val="139439016"/>
+        <c:axId val="140211336"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1800,11 +1800,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142206176"/>
-        <c:axId val="142203432"/>
+        <c:axId val="140211728"/>
+        <c:axId val="140212904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142205784"/>
+        <c:axId val="139439016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1861,12 +1861,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142202256"/>
+        <c:crossAx val="140211336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142202256"/>
+        <c:axId val="140211336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1923,12 +1923,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142205784"/>
+        <c:crossAx val="139439016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142203432"/>
+        <c:axId val="140212904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,12 +1971,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142206176"/>
+        <c:crossAx val="140211728"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142206176"/>
+        <c:axId val="140211728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1986,7 +1986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142203432"/>
+        <c:crossAx val="140212904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2082,7 +2082,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5268,11 +5267,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142201080"/>
-        <c:axId val="142204216"/>
+        <c:axId val="140213296"/>
+        <c:axId val="141764848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142201080"/>
+        <c:axId val="140213296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5329,12 +5328,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142204216"/>
+        <c:crossAx val="141764848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142204216"/>
+        <c:axId val="141764848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5391,7 +5390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="142201080"/>
+        <c:crossAx val="140213296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5405,7 +5404,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7967,7 +7965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -12660,9 +12658,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -13153,7 +13151,7 @@
         <v>409</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -13173,10 +13171,10 @@
         <v>412</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -13193,7 +13191,7 @@
         <v>409</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
@@ -13653,7 +13651,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -13670,7 +13668,7 @@
         <v>277</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>